<commit_message>
displaying coach on export, fixed contestant coach id
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/result_template.xlsx
+++ b/src/main/resources/templates/result_template.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Név</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>${member.name}</t>
-  </si>
-  <si>
-    <t>Eredménylista</t>
   </si>
   <si>
     <t>${contestant.age}</t>
@@ -191,6 +188,12 @@
   </si>
   <si>
     <t>${member.positionString}</t>
+  </si>
+  <si>
+    <t>${result.individualCategory.coach}</t>
+  </si>
+  <si>
+    <t>${result.teamCategory.coach}</t>
   </si>
 </sst>
 </file>
@@ -508,6 +511,24 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -537,24 +558,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -980,7 +983,7 @@
   <dimension ref="A1:O1215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H5" sqref="H5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,64 +1004,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
-        <v>16</v>
+      <c r="A1" s="29" t="s">
+        <v>15</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="29" t="s">
-        <v>16</v>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="35" t="s">
+        <v>15</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="43" t="s">
-        <v>18</v>
+      <c r="A2" s="33" t="s">
+        <v>17</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="31" t="s">
-        <v>18</v>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="37" t="s">
+        <v>17</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>17</v>
+      <c r="A3" s="34" t="s">
+        <v>16</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="35" t="s">
-        <v>17</v>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="41" t="s">
+        <v>16</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -1070,7 +1073,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1083,26 +1086,26 @@
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42" t="s">
-        <v>12</v>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32" t="s">
+        <v>25</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="33" t="s">
+      <c r="E5" s="32"/>
+      <c r="F5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="37" t="s">
-        <v>12</v>
+      <c r="G5" s="40"/>
+      <c r="H5" s="43" t="s">
+        <v>26</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
       <c r="M5" s="11"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
@@ -1110,19 +1113,19 @@
     <row r="6" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>1</v>
@@ -1131,10 +1134,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>3</v>
@@ -1148,7 +1151,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>6</v>
@@ -1157,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>8</v>
@@ -1166,19 +1169,19 @@
         <v>10</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="K7" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>25</v>
       </c>
       <c r="L7" s="21" t="s">
         <v>9</v>
@@ -1194,7 +1197,7 @@
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -21727,16 +21730,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="H5:L5"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F3:L3"/>
-    <mergeCell ref="H5:L5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
renamed Coach to Supervisor to better incorporate type
Signed-off-by: Balázs Dániel <shockrifle666@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/result_template.xlsx
+++ b/src/main/resources/templates/result_template.xlsx
@@ -133,13 +133,13 @@
     <t xml:space="preserve">${result.individualCategory.name}</t>
   </si>
   <si>
-    <t xml:space="preserve">${result.individualCategory.coach}</t>
+    <t xml:space="preserve">${result.individualCategory.supervisor}</t>
   </si>
   <si>
     <t xml:space="preserve">${result.teamCategory.name}</t>
   </si>
   <si>
-    <t xml:space="preserve">${result.teamCategory.coach}</t>
+    <t xml:space="preserve">${result.teamCategory.supervisor}</t>
   </si>
   <si>
     <t xml:space="preserve">Rajtsz.</t>
@@ -628,9 +628,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3089160</xdr:colOff>
+      <xdr:colOff>3088800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -643,8 +643,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4450320" y="636480"/>
-          <a:ext cx="2005560" cy="1204920"/>
+          <a:off x="4450680" y="636480"/>
+          <a:ext cx="2005200" cy="1204560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -665,9 +665,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>509400</xdr:colOff>
+      <xdr:colOff>509040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>405360</xdr:rowOff>
+      <xdr:rowOff>405000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -680,8 +680,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11845440" y="570960"/>
-          <a:ext cx="2005200" cy="1206000"/>
+          <a:off x="11846160" y="570960"/>
+          <a:ext cx="2004120" cy="1205640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -704,23 +704,23 @@
   <dimension ref="A1:O1008"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.54"/>
   </cols>
   <sheetData>

</xml_diff>